<commit_message>
Handled an error caused by empty url provided to the `get_response_code(url)` function
</commit_message>
<xml_diff>
--- a/Twitter Data.xlsx
+++ b/Twitter Data.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="Output" sheetId="3" r:id="rId2"/>
-    <sheet name="Errors" sheetId="2" r:id="rId3"/>
+    <sheet name="Output" sheetId="2" r:id="rId2"/>
+    <sheet name="Errors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -30,69 +30,63 @@
     <t>dailystarnews</t>
   </si>
   <si>
-    <t xml:space="preserve">Failed to get the final url for </t>
+    <t>SiyamAh66347457</t>
+  </si>
+  <si>
+    <t>Screen Name</t>
+  </si>
+  <si>
+    <t>Name / ID</t>
+  </si>
+  <si>
+    <t>Followers</t>
+  </si>
+  <si>
+    <t>Following</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Joined Date</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>Resolution Days 2021 is here to make a Revolution! Check it out Now!</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>https://t.co/INfSv8tvj9</t>
+  </si>
+  <si>
+    <t>17 July 2009</t>
+  </si>
+  <si>
+    <t>Bangladesh Cricket</t>
+  </si>
+  <si>
+    <t>The Official Twitter of Bangladesh Cricket.</t>
+  </si>
+  <si>
+    <t>SBNCS, Mirpur-2, Dhaka-1216</t>
   </si>
   <si>
     <t>https://t.co/bCwTBCUXj7</t>
   </si>
   <si>
-    <t>Due to</t>
-  </si>
-  <si>
-    <t>HTTPSConnectionPool(host='www.tigercricket.com.bd', port=443): Max retries exceeded with url: / (Caused by NewConnectionError('&lt;urllib3.connection.HTTPSConnection object at 0x000002C1CD443790&gt;: Failed to establish a new connection: [WinError 10060] A connection attempt failed because the connected party did not properly respond after a period of time, or established connection failed because connected host has failed to respond'))</t>
-  </si>
-  <si>
-    <t>Screen Name</t>
-  </si>
-  <si>
-    <t>Name / ID</t>
-  </si>
-  <si>
-    <t>Followers</t>
-  </si>
-  <si>
-    <t>Following</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Joined Date</t>
-  </si>
-  <si>
-    <t>Verified</t>
-  </si>
-  <si>
-    <t>GeeksforGeeks</t>
-  </si>
-  <si>
-    <t>Your friendly neighborhood assignment helper</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>https://practice.geeksforgeeks.org/courses</t>
-  </si>
-  <si>
-    <t>17 July 2009</t>
-  </si>
-  <si>
-    <t>Bangladesh Cricket</t>
-  </si>
-  <si>
-    <t>The Official Twitter of Bangladesh Cricket.</t>
-  </si>
-  <si>
-    <t>SBNCS, Mirpur-2, Dhaka-1216</t>
-  </si>
-  <si>
     <t>13 June 2011</t>
   </si>
   <si>
@@ -109,13 +103,19 @@
   </si>
   <si>
     <t>27 September 2009</t>
+  </si>
+  <si>
+    <t>Siyam Ahmed</t>
+  </si>
+  <si>
+    <t>29 September 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +136,12 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF8899A6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -175,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -184,7 +190,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -519,6 +526,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -527,7 +539,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" topLeftCell="I1" activePane="topRight" state="frozen"/>
@@ -540,32 +552,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -573,25 +585,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2">
-        <v>22382</v>
+        <v>22702</v>
       </c>
       <c r="D2">
         <v>48</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
@@ -602,25 +614,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>2624960</v>
+        <v>2628515</v>
       </c>
       <c r="D3">
         <v>41</v>
       </c>
       <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -631,28 +643,48 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>860611</v>
+      </c>
+      <c r="D4">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="C4">
-        <v>858179</v>
-      </c>
-      <c r="D4">
-        <v>80</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -662,33 +694,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>